<commit_message>
Updated and refactored the graphing and summarizing. changed default to 1.8% daily yield from LPing
</commit_message>
<xml_diff>
--- a/summary_7d.xlsx
+++ b/summary_7d.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\GitHub\GitHub\DefiTuna_PDN_Ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC4A0CD-38F1-48BF-BEC2-0C448BCB9BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2129A287-648F-4167-A8A9-1B5F18CF4C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{78543B86-A795-403C-AAA7-CCC8E0E47F0F}"/>
+    <workbookView xWindow="12720" yWindow="0" windowWidth="12960" windowHeight="13760" xr2:uid="{78543B86-A795-403C-AAA7-CCC8E0E47F0F}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_7d" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Initial Total Debt Value</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>0.5 SOL HODL Return</t>
+  </si>
+  <si>
+    <t>SOL Price</t>
   </si>
 </sst>
 </file>
@@ -741,13 +744,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -755,6 +751,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1130,464 +1135,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72AADA3D-F136-4963-8039-2B2006F6582F}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="B1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="2:22" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A2" s="6">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.5">
+      <c r="B3" s="3">
         <v>180</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C3" s="2">
         <v>1.52</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D3" s="2">
         <v>273.33</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G3" s="2">
         <v>273.33</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H3" s="2">
         <v>0.75</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I3" s="2">
         <v>50</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J3" s="2">
         <v>135</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K3" s="2">
         <v>50</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L3" s="2">
         <v>185</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M3" s="2">
         <v>88.33</v>
       </c>
-      <c r="M2" s="2">
-        <v>276.99</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="N3" s="2">
+        <v>309.69</v>
+      </c>
+      <c r="O3" s="2">
         <v>186.2</v>
       </c>
-      <c r="O2" s="2">
-        <v>90.79</v>
-      </c>
-      <c r="P2" s="2">
+      <c r="P3" s="2">
+        <v>123.49</v>
+      </c>
+      <c r="Q3" s="2">
         <v>0.77</v>
       </c>
-      <c r="Q2" s="2">
-        <v>-9.2100000000000009</v>
-      </c>
-      <c r="R2" s="2">
+      <c r="R3" s="2">
+        <v>23.49</v>
+      </c>
+      <c r="S3" s="2">
         <v>90</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T3" s="2">
         <v>-10</v>
       </c>
-      <c r="T2" s="2">
-        <v>0.78</v>
-      </c>
-      <c r="U2" s="7">
+      <c r="U3" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="V3" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A3" s="8">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.5">
+      <c r="B4" s="5">
         <v>185</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>1.52</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>280.93</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>280.93</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="H3" s="1">
-        <v>50</v>
-      </c>
-      <c r="I3" s="1">
-        <v>138.75</v>
-      </c>
-      <c r="J3" s="1">
-        <v>50</v>
-      </c>
-      <c r="K3" s="1">
-        <v>188.75</v>
-      </c>
-      <c r="L3" s="1">
-        <v>92.18</v>
-      </c>
-      <c r="M3" s="1">
-        <v>284.69</v>
-      </c>
-      <c r="N3" s="1">
-        <v>189.97</v>
-      </c>
-      <c r="O3" s="1">
-        <v>94.71</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>-5.29</v>
-      </c>
-      <c r="R3" s="1">
-        <v>92.5</v>
-      </c>
-      <c r="S3" s="1">
-        <v>-7.5</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="U3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A4" s="8">
-        <v>190</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.52</v>
-      </c>
-      <c r="C4" s="1">
-        <v>288.52</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>280.93</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="1">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1">
+        <v>138.75</v>
+      </c>
+      <c r="K4" s="1">
+        <v>50</v>
+      </c>
+      <c r="L4" s="1">
+        <v>188.75</v>
+      </c>
+      <c r="M4" s="1">
+        <v>92.18</v>
+      </c>
+      <c r="N4" s="1">
+        <v>318.29000000000002</v>
+      </c>
+      <c r="O4" s="1">
+        <v>189.97</v>
+      </c>
+      <c r="P4" s="1">
+        <v>128.32</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="R4" s="1">
+        <v>28.32</v>
+      </c>
+      <c r="S4" s="1">
+        <v>92.5</v>
+      </c>
+      <c r="T4" s="1">
+        <v>-7.5</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.5">
+      <c r="B5" s="5">
+        <v>190</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.52</v>
+      </c>
+      <c r="D5" s="1">
         <v>288.52</v>
       </c>
-      <c r="G4" s="1">
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>288.52</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.75</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I5" s="1">
         <v>50</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J5" s="1">
         <v>142.5</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K5" s="1">
         <v>50</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L5" s="1">
         <v>192.5</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M5" s="1">
         <v>96.02</v>
       </c>
-      <c r="M4" s="1">
-        <v>292.38</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="N5" s="1">
+        <v>326.89999999999998</v>
+      </c>
+      <c r="O5" s="1">
         <v>193.75</v>
       </c>
-      <c r="O4" s="1">
-        <v>98.63</v>
-      </c>
-      <c r="P4" s="1">
+      <c r="P5" s="1">
+        <v>133.15</v>
+      </c>
+      <c r="Q5" s="1">
         <v>0.77</v>
       </c>
-      <c r="Q4" s="1">
-        <v>-1.37</v>
-      </c>
-      <c r="R4" s="1">
+      <c r="R5" s="1">
+        <v>33.15</v>
+      </c>
+      <c r="S5" s="1">
         <v>95</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T5" s="1">
         <v>-5</v>
       </c>
-      <c r="T4" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="U4" s="9">
+      <c r="U5" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="V5" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A5" s="8">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.5">
+      <c r="B6" s="5">
+        <v>195</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>223.56</v>
+      </c>
+      <c r="E6" s="1">
+        <v>71.709999999999994</v>
+      </c>
+      <c r="F6" s="1">
+        <v>71.709999999999994</v>
+      </c>
+      <c r="G6" s="1">
+        <v>295.27</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I6" s="1">
+        <v>50</v>
+      </c>
+      <c r="J6" s="1">
+        <v>146.25</v>
+      </c>
+      <c r="K6" s="1">
+        <v>50</v>
+      </c>
+      <c r="L6" s="1">
+        <v>196.25</v>
+      </c>
+      <c r="M6" s="1">
+        <v>99.02</v>
+      </c>
+      <c r="N6" s="1">
+        <v>334.54</v>
+      </c>
+      <c r="O6" s="1">
+        <v>197.52</v>
+      </c>
+      <c r="P6" s="1">
+        <v>137.02000000000001</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="R6" s="1">
+        <v>37.020000000000003</v>
+      </c>
+      <c r="S6" s="1">
+        <v>97.5</v>
+      </c>
+      <c r="T6" s="1">
+        <v>-2.5</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="V6" s="6">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.5">
+      <c r="B7" s="5">
         <v>200</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C7" s="1">
         <v>0.75</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D7" s="1">
         <v>150</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E7" s="1">
         <v>150</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F7" s="1">
         <v>150</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G7" s="1">
         <v>300</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H7" s="1">
         <v>0.75</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I7" s="1">
         <v>50</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J7" s="1">
         <v>150</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K7" s="1">
         <v>50</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L7" s="1">
         <v>200</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M7" s="1">
         <v>100</v>
       </c>
-      <c r="M5" s="1">
-        <v>304.01</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="N7" s="1">
+        <v>339.9</v>
+      </c>
+      <c r="O7" s="1">
         <v>201.29</v>
       </c>
-      <c r="O5" s="1">
-        <v>102.72</v>
-      </c>
-      <c r="P5" s="1">
+      <c r="P7" s="1">
+        <v>138.61000000000001</v>
+      </c>
+      <c r="Q7" s="1">
         <v>0</v>
       </c>
-      <c r="Q5" s="1">
-        <v>2.72</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="R7" s="1">
+        <v>38.61</v>
+      </c>
+      <c r="S7" s="1">
         <v>100</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T7" s="1">
         <v>0</v>
       </c>
-      <c r="T5" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="U5" s="9">
+      <c r="U7" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="V7" s="6">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.5">
+      <c r="B8" s="5">
+        <v>205</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="D8" s="1">
+        <v>75.47</v>
+      </c>
+      <c r="E8" s="1">
+        <v>227.32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>227.32</v>
+      </c>
+      <c r="G8" s="1">
+        <v>302.79000000000002</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I8" s="1">
+        <v>50</v>
+      </c>
+      <c r="J8" s="1">
+        <v>153.75</v>
+      </c>
+      <c r="K8" s="1">
+        <v>50</v>
+      </c>
+      <c r="L8" s="1">
+        <v>203.75</v>
+      </c>
+      <c r="M8" s="1">
+        <v>99.04</v>
+      </c>
+      <c r="N8" s="1">
+        <v>343.06</v>
+      </c>
+      <c r="O8" s="1">
+        <v>205.07</v>
+      </c>
+      <c r="P8" s="1">
+        <v>138</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>-0.38</v>
+      </c>
+      <c r="R8" s="1">
+        <v>38</v>
+      </c>
+      <c r="S8" s="1">
+        <v>102.5</v>
+      </c>
+      <c r="T8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="U8" s="1">
+        <v>-0.34</v>
+      </c>
+      <c r="V8" s="6">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A6" s="8">
-        <v>205</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.37</v>
-      </c>
-      <c r="C6" s="1">
-        <v>75.47</v>
-      </c>
-      <c r="D6" s="1">
-        <v>227.32</v>
-      </c>
-      <c r="E6" s="1">
-        <v>227.32</v>
-      </c>
-      <c r="F6" s="1">
-        <v>302.79000000000002</v>
-      </c>
-      <c r="G6" s="1">
+    <row r="9" spans="2:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="7">
+        <v>210</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>303.7</v>
+      </c>
+      <c r="F9" s="8">
+        <v>303.7</v>
+      </c>
+      <c r="G9" s="8">
+        <v>303.7</v>
+      </c>
+      <c r="H9" s="8">
         <v>0.75</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I9" s="8">
         <v>50</v>
       </c>
-      <c r="I6" s="1">
-        <v>153.75</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="J9" s="8">
+        <v>157.5</v>
+      </c>
+      <c r="K9" s="8">
         <v>50</v>
       </c>
-      <c r="K6" s="1">
-        <v>203.75</v>
-      </c>
-      <c r="L6" s="1">
-        <v>99.04</v>
-      </c>
-      <c r="M6" s="1">
-        <v>306.83999999999997</v>
-      </c>
-      <c r="N6" s="1">
-        <v>205.07</v>
-      </c>
-      <c r="O6" s="1">
-        <v>101.77</v>
-      </c>
-      <c r="P6" s="1">
-        <v>-0.38</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1.77</v>
-      </c>
-      <c r="R6" s="1">
-        <v>102.5</v>
-      </c>
-      <c r="S6" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="T6" s="1">
-        <v>-0.38</v>
-      </c>
-      <c r="U6" s="9">
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10">
-        <v>210</v>
-      </c>
-      <c r="B7" s="11">
-        <v>0</v>
-      </c>
-      <c r="C7" s="11">
-        <v>0</v>
-      </c>
-      <c r="D7" s="11">
-        <v>303.7</v>
-      </c>
-      <c r="E7" s="11">
-        <v>303.7</v>
-      </c>
-      <c r="F7" s="11">
-        <v>303.7</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="H7" s="11">
-        <v>50</v>
-      </c>
-      <c r="I7" s="11">
-        <v>157.5</v>
-      </c>
-      <c r="J7" s="11">
-        <v>50</v>
-      </c>
-      <c r="K7" s="11">
+      <c r="L9" s="8">
         <v>207.5</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M9" s="8">
         <v>96.2</v>
       </c>
-      <c r="M7" s="11">
-        <v>307.77</v>
-      </c>
-      <c r="N7" s="11">
+      <c r="N9" s="8">
+        <v>344.1</v>
+      </c>
+      <c r="O9" s="8">
         <v>208.84</v>
       </c>
-      <c r="O7" s="11">
-        <v>98.93</v>
-      </c>
-      <c r="P7" s="11">
+      <c r="P9" s="8">
+        <v>135.26</v>
+      </c>
+      <c r="Q9" s="8">
         <v>-0.75</v>
       </c>
-      <c r="Q7" s="11">
-        <v>-1.07</v>
-      </c>
-      <c r="R7" s="11">
+      <c r="R9" s="8">
+        <v>35.26</v>
+      </c>
+      <c r="S9" s="8">
         <v>105</v>
       </c>
-      <c r="S7" s="11">
+      <c r="T9" s="8">
         <v>5</v>
       </c>
-      <c r="T7" s="11">
+      <c r="U9" s="8">
         <v>-0.75</v>
       </c>
-      <c r="U7" s="12">
+      <c r="V9" s="9">
         <v>-0.04</v>
       </c>
     </row>

</xml_diff>